<commit_message>
Update Flashcards: Double backs
</commit_message>
<xml_diff>
--- a/other_resources/old_excel_files/VOK_Kap1_La nature et la géo._V2.xlsx
+++ b/other_resources/old_excel_files/VOK_Kap1_La nature et la géo._V2.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="244">
   <si>
     <t xml:space="preserve">Typ</t>
   </si>
@@ -931,7 +931,7 @@
   <dimension ref="A1:E116"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A76" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B48" activeCellId="0" sqref="B48"/>
+      <selection pane="topLeft" activeCell="A110" activeCellId="0" sqref="A110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2349,7 +2349,10 @@
         <v>241</v>
       </c>
     </row>
-    <row r="116" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="116" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A116" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="B116" s="1" t="s">
         <v>242</v>
       </c>

</xml_diff>